<commit_message>
Further tests using different cross validation splits
</commit_message>
<xml_diff>
--- a/src/Gabriel/ML_Workbook_1/Findings/Classification Ranking.xlsx
+++ b/src/Gabriel/ML_Workbook_1/Findings/Classification Ranking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="74">
   <si>
     <t>Accuracy</t>
   </si>
@@ -227,6 +227,18 @@
   </si>
   <si>
     <t>80/20%</t>
+  </si>
+  <si>
+    <t>70/30%</t>
+  </si>
+  <si>
+    <t>75/25%</t>
+  </si>
+  <si>
+    <t>85/15%</t>
+  </si>
+  <si>
+    <t>90/10%</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K132"/>
+  <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D106" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,10 +2633,10 @@
         <v>1</v>
       </c>
       <c r="I127" s="2">
-        <v>0.93491321762299995</v>
+        <v>0.93558077436599996</v>
       </c>
       <c r="J127" s="2">
-        <v>0.93472719932500004</v>
+        <v>0.93539079920099999</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -2632,23 +2644,251 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>18</v>
+      </c>
+      <c r="B133" t="s">
+        <v>51</v>
+      </c>
+      <c r="C133" t="s">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133" t="s">
+        <v>3</v>
+      </c>
+      <c r="F133" t="s">
+        <v>70</v>
+      </c>
+      <c r="G133" t="s">
+        <v>61</v>
+      </c>
+      <c r="H133" t="s">
+        <v>1</v>
+      </c>
+      <c r="I133" s="2">
+        <v>0.92677498330700003</v>
+      </c>
+      <c r="J133" s="2">
+        <v>0.92655824004300003</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>19</v>
+      </c>
+      <c r="B139" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139" t="s">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139" t="s">
+        <v>3</v>
+      </c>
+      <c r="F139" t="s">
+        <v>71</v>
+      </c>
+      <c r="G139" t="s">
+        <v>61</v>
+      </c>
+      <c r="H139" t="s">
+        <v>1</v>
+      </c>
+      <c r="I139" s="2">
+        <v>0.93135683760700005</v>
+      </c>
+      <c r="J139" s="2">
+        <v>0.93114810886300003</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>20</v>
+      </c>
+      <c r="B145" t="s">
+        <v>51</v>
+      </c>
+      <c r="C145" t="s">
+        <v>3</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145" t="s">
+        <v>3</v>
+      </c>
+      <c r="F145" t="s">
+        <v>73</v>
+      </c>
+      <c r="G145" t="s">
+        <v>61</v>
+      </c>
+      <c r="H145" t="s">
+        <v>1</v>
+      </c>
+      <c r="I145" s="2">
+        <v>0.93457943925200004</v>
+      </c>
+      <c r="J145" s="2">
+        <v>0.93435051452899998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>21</v>
+      </c>
+      <c r="B151" t="s">
+        <v>51</v>
+      </c>
+      <c r="C151" t="s">
+        <v>3</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151" t="s">
+        <v>3</v>
+      </c>
+      <c r="F151" t="s">
+        <v>72</v>
+      </c>
+      <c r="G151" t="s">
+        <v>61</v>
+      </c>
+      <c r="H151" t="s">
+        <v>1</v>
+      </c>
+      <c r="I151" s="2">
+        <v>0.93368936359599997</v>
+      </c>
+      <c r="J151" s="2">
+        <v>0.93347648280700002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>